<commit_message>
Anjana's diary entry for last week
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\Reverse Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D2A3A-1466-422F-9537-51DE35D4F47E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1DDE2-E050-4635-854D-DC61A69D962D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -173,6 +173,37 @@
 Practiced few techniques using JPacMan source code by fixing bugs and making small functional changes.
 Got to know how the process of reverse engineering works in the industry and Google in particular.
 </t>
+  </si>
+  <si>
+    <t>Work on the homework (individual) practice questions.</t>
+  </si>
+  <si>
+    <t>Explored JPacMan3 project and figured out the answers to the questions. Used opportunist approach followed by bottom up approach in order to read and understand the code.
+Included the findings in a document.</t>
+  </si>
+  <si>
+    <t>Since there was enough comments, it was easier to read and understand the code. Understood the importance of having comments in improving the readability of the code.</t>
+  </si>
+  <si>
+    <t>7pm - 9pm</t>
+  </si>
+  <si>
+    <t>Look forward to practice more and improve my code reading skills.</t>
+  </si>
+  <si>
+    <t>6pm-10pm</t>
+  </si>
+  <si>
+    <t>Still feeling nervous about the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narrowing down one project from a list of possible options was more difficult that expected. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explored various open source projects available on GitHub, selected OpenRefine and submitted the pull request. </t>
+  </si>
+  <si>
+    <t>Select an open source project on GitHub</t>
   </si>
 </sst>
 </file>
@@ -666,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,23 +930,51 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
+    <row r="15" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>43847</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>43848</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>

</xml_diff>

<commit_message>
Anjana's diary entry for 1/23
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\Reverse Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1DDE2-E050-4635-854D-DC61A69D962D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF8916-6805-4452-906A-7B56F2BB23C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -205,12 +205,31 @@
   <si>
     <t>Select an open source project on GitHub</t>
   </si>
+  <si>
+    <t>5pm-7.50pm</t>
+  </si>
+  <si>
+    <t>Understood how UML can help in reading and understanding the code</t>
+  </si>
+  <si>
+    <t>Learn new concepts and practice more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This week's homework looks quite challenging. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about the concept of mental models, its properties, how it applies in software and its limitations
+Discussed the ways in which we can externalize mental models while reading the code
+Tried to figure out where in code a particular feature has been implemented by - 1) using a template  2) using UML
+Understood the different techniques that software engineers in the industry use to read the code like diagrams, notes and going through the tests
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +321,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -342,7 +369,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -377,6 +404,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -695,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,146 +869,104 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>43840</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>27</v>
-      </c>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
+        <v>43840</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <v>43843</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="78" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="156" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
-        <v>43846</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
-        <v>43847</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
-        <v>43848</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -985,50 +974,92 @@
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+    <row r="18" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>43846</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+    <row r="20" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>43847</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
+    <row r="22" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>43848</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
@@ -1039,20 +1070,34 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
+    <row r="24" spans="1:7" s="13" customFormat="1" ht="280.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>43853</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
@@ -1061,7 +1106,7 @@
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="D26" s="8"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
@@ -1070,7 +1115,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
@@ -1079,7 +1124,7 @@
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="D28" s="8"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
@@ -1965,6 +2010,60 @@
       <c r="E126" s="7"/>
       <c r="F126" s="7"/>
       <c r="G126" s="8"/>
+    </row>
+    <row r="127" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="7"/>
+      <c r="B127" s="7"/>
+      <c r="C127" s="7"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7"/>
+      <c r="G127" s="8"/>
+    </row>
+    <row r="128" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="7"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
+      <c r="G128" s="8"/>
+    </row>
+    <row r="129" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
+      <c r="G129" s="8"/>
+    </row>
+    <row r="130" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="7"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
+      <c r="G130" s="8"/>
+    </row>
+    <row r="131" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="7"/>
+      <c r="G131" s="8"/>
+    </row>
+    <row r="132" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="7"/>
+      <c r="G132" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Anjana's diary entry for 1/30
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\Reverse Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF8916-6805-4452-906A-7B56F2BB23C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5094AA97-B3ED-43C1-ACF7-DD82C2F7BFA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -223,6 +223,66 @@
 Tried to figure out where in code a particular feature has been implemented by - 1) using a template  2) using UML
 Understood the different techniques that software engineers in the industry use to read the code like diagrams, notes and going through the tests
 </t>
+  </si>
+  <si>
+    <t>See if we can select a new open source project</t>
+  </si>
+  <si>
+    <t>We were happy when our pull request got accepted</t>
+  </si>
+  <si>
+    <t>Since we had doubts regarding the project that was initially selected, we decided to try look for more options and to find a new project that is more challenging and interesting than the initial one. We all liked h2 database project and thought it would be interesting to work on databases. Therefore we submitted a new pull request. We also tried to build the project once before submitting the pull request.</t>
+  </si>
+  <si>
+    <t>Deciding which project to work on was difficult</t>
+  </si>
+  <si>
+    <t>12pm - 3pm</t>
+  </si>
+  <si>
+    <t>8pm - 10pm</t>
+  </si>
+  <si>
+    <t>Start working on this week's homework</t>
+  </si>
+  <si>
+    <t>The UML diagram of the project is really huge and has so many connections between the classes. Trying to analyze it on the whole can be a pretty challenging task</t>
+  </si>
+  <si>
+    <t>We were still clueless about how to start looking for the implementation of the feature.</t>
+  </si>
+  <si>
+    <t>10pm - 1 am</t>
+  </si>
+  <si>
+    <t>Continue working on the homework</t>
+  </si>
+  <si>
+    <t>Prepare the report</t>
+  </si>
+  <si>
+    <t>We prepared a report that explains our search approach/strategy by making use of the templates</t>
+  </si>
+  <si>
+    <t>Templates were helpful while writing the report</t>
+  </si>
+  <si>
+    <t>As the project was approved, we started working on this week's homework. Before starting off, I explained the concepts taught in the previous class to Aman since he was not present that day. After that we created UML diagram for the project on IntelliJ. We also decided to analyze Create Table and set user privilege features in detail for the homework.</t>
+  </si>
+  <si>
+    <t>We analysed the selected features using find usage functionality on Intellij to look for possible classes and methods. We also used the templates to keep track of the relevant files we visited. We were also able to figure out where these classes are present in the UML diagram</t>
+  </si>
+  <si>
+    <t>It took a lot of time to figure out where the features are implemented in the code. Templates helped in keeping track of what we were doing</t>
+  </si>
+  <si>
+    <t>Neutral, we think we found relevant classes and methods, but there could be something that we missed out</t>
+  </si>
+  <si>
+    <t>10am - 1pm</t>
+  </si>
+  <si>
+    <t>Happy to complete the homework</t>
   </si>
 </sst>
 </file>
@@ -401,13 +461,13 @@
     <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -728,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,24 +798,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1070,14 +1130,14 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" s="13" customFormat="1" ht="280.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="280.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>43853</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -1102,17 +1162,31 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
+    <row r="26" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>43856</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
@@ -1120,14 +1194,28 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
+    <row r="28" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>43856</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
@@ -1138,14 +1226,28 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
+    <row r="30" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
+        <v>43858</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
@@ -1156,14 +1258,28 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8"/>
+    <row r="32" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>

</xml_diff>

<commit_message>
Anjana's diary entry for week 4
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\Reverse Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5094AA97-B3ED-43C1-ACF7-DD82C2F7BFA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3FC80B-6650-4DE7-A349-B717AF629369}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -283,6 +283,85 @@
   </si>
   <si>
     <t>Happy to complete the homework</t>
+  </si>
+  <si>
+    <t>Learn more concepts and practice the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about key expert practices,structural vs behavioral models, UML,call graphs, sequence diagrams etc. </t>
+  </si>
+  <si>
+    <t>Understood the importance of focusing on the core essence of the system rather than the extra functionalities, going deeper into the code base as when needed and how working with others can help us</t>
+  </si>
+  <si>
+    <t>Happy to learn different ways to model code</t>
+  </si>
+  <si>
+    <t>11:00 am - 1:00pm and 9:30 pm - 11:00 pm</t>
+  </si>
+  <si>
+    <t>Aman, Vaishakhi</t>
+  </si>
+  <si>
+    <t>Decide two features for the homework and start working on it.</t>
+  </si>
+  <si>
+    <t>We decided two features: 
+1. how does the h2 database support embedded and server mode
+2. How is data actually persisted from h2 onto our disk.
+We were also able to figure out the implementation of the first feature</t>
+  </si>
+  <si>
+    <t>We were facing some issues with running our application because Tools.jar file was not being detected in pom.xml. So we had to downgrade our java version, edit the system path in pom.xml to reflect the location of tools.jar and do a maven clean.
+Since the code uses proper naming conventions it was much easier to read the codebase.</t>
+  </si>
+  <si>
+    <t>Was little frustrated initially when we were not able to run the system. Happy to have figured out the first feature</t>
+  </si>
+  <si>
+    <t>10pm - 12pm</t>
+  </si>
+  <si>
+    <t>Figure out second feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some features are very difficult to figure out </t>
+  </si>
+  <si>
+    <t>We were not able to figure out our second feature, even after spending a lot of time and doing a lot of debugging Hence we decided to choose a different feature as our second option which was "How does H2 database handle multiple commands like Insert/Delete etc"</t>
+  </si>
+  <si>
+    <t>Slightly nervous if we will be able to complete the homework or not</t>
+  </si>
+  <si>
+    <t>10pm - 2am</t>
+  </si>
+  <si>
+    <t>Finish working on second feature</t>
+  </si>
+  <si>
+    <t>Able to understand the flow and we could draw the diagrams</t>
+  </si>
+  <si>
+    <t>It was difficult and had to spend so much time</t>
+  </si>
+  <si>
+    <t>Relaxed as we were able to finally finish the second feature</t>
+  </si>
+  <si>
+    <t>10am-12.30pm</t>
+  </si>
+  <si>
+    <t>Prepare reports</t>
+  </si>
+  <si>
+    <t>Finished writing the reports</t>
+  </si>
+  <si>
+    <t>Since we have prepared the flow digrams while looking at the code, it was easier to write the report</t>
+  </si>
+  <si>
+    <t>Happy to finish the homework</t>
   </si>
 </sst>
 </file>
@@ -788,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,17 +1360,31 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8"/>
+    <row r="33" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1299,14 +1392,28 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
+    <row r="35" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
@@ -1317,14 +1424,28 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
+    <row r="37" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
@@ -1335,14 +1456,28 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
+    <row r="39" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
@@ -1353,14 +1488,28 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
+    <row r="41" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="10">
+        <v>43867</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>

</xml_diff>

<commit_message>
Anjana's diary entry for week 6
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF79AA3-BE84-43BB-A340-CC857AB38498}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A1C2F-32B9-4038-BCFD-4579A75B3C22}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -374,6 +374,55 @@
   </si>
   <si>
     <t>Looking forward to prepare for the mid term exam next week.</t>
+  </si>
+  <si>
+    <t>Mid term exam</t>
+  </si>
+  <si>
+    <t>Gave the mid-term exam. Was able to answer all the questions. 
+Learned more key expert practices and what is meant by the big picture of a system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to improve my time management skills while writing the exam as I had to rush through at the end because I didn't plan my time properly from the beginning.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking forward to the results of the mid term exam. </t>
+  </si>
+  <si>
+    <t>11am - 2pm</t>
+  </si>
+  <si>
+    <t>Worked on home work 1 and tried to improve the report based on Kaj's feedback. Resubmitted the homework 1
+Started working on the third homework by searching for the necessary information required to prepare the report</t>
+  </si>
+  <si>
+    <t>Resubmit homework 1
+Start working on homework 3</t>
+  </si>
+  <si>
+    <t>I could clearly see the differences in the first and second versions of our home work 1 report as we tried to explained the feature and our approch in detail. Diving a little bit more deeper helped in bridging the gaps in explaining the features and our approach.</t>
+  </si>
+  <si>
+    <t>11pm - 12 am</t>
+  </si>
+  <si>
+    <t>Vaishakhi,Aman</t>
+  </si>
+  <si>
+    <t>Finish homework 3</t>
+  </si>
+  <si>
+    <t>We prepared the report for the homework after gathering all necessary information regarding the Big Picture of the system.</t>
+  </si>
+  <si>
+    <t>Feeling great after resubmitting homework1</t>
+  </si>
+  <si>
+    <t>Happy to finish homework 3</t>
+  </si>
+  <si>
+    <t>Realized the importance and impact of the system in terms of the number of companies and the industries in which it is currently being used. It would be amazing if we are able to solve atleast one open issue.</t>
   </si>
 </sst>
 </file>
@@ -879,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D48" zoomScale="120" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,14 +1613,28 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
+    <row r="45" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="10">
+        <v>43874</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
@@ -1582,14 +1645,28 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
+    <row r="47" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="10">
+        <v>43877</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
@@ -1600,14 +1677,28 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
+    <row r="49" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="10">
+        <v>43880</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>

</xml_diff>

<commit_message>
Anjana's diary entry for week 7 (#407)
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A1C2F-32B9-4038-BCFD-4579A75B3C22}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13116804-7342-4717-A6AE-6EA63837BD4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="135">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -423,6 +423,53 @@
   </si>
   <si>
     <t>Realized the importance and impact of the system in terms of the number of companies and the industries in which it is currently being used. It would be amazing if we are able to solve atleast one open issue.</t>
+  </si>
+  <si>
+    <t>Was expecting mid-term results, looking forward to know more about the system architecture</t>
+  </si>
+  <si>
+    <t>Learned three new Key Expert practices.
+Learned about the architecture of the system and the process of understanding the architecture from source code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there's no proper documented architecture, the first step in understanding the architecture from the source code is by looking at the folder/package  structure and trying to grouping various related classes together. We can start with the UML diagram and slowly try to abstract up. 
+Pull requests can also be a useful tool as lot of design decisions could be present in pull requests which will help us to understand the rationale of the developer and why certain things are written in a certain way. </t>
+  </si>
+  <si>
+    <t>This week's homework is pretty vast and have to start working on it soon.</t>
+  </si>
+  <si>
+    <t>Understood both the as-described and as-implemented architecture of the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realized the importance of having a documented version of architecture as it helps developers in the future 
+There are only few variations in the as-described and as-implemented architectures of h2, which means the h2 community has done a really good job at code reviews and maintaining the standards
+</t>
+  </si>
+  <si>
+    <t>Proud to complete the most challenging part of this week's assignment</t>
+  </si>
+  <si>
+    <t>Understand the architecture of the system and document the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish the remaining sections of the homework like pull requests, issues, state of the system etc. </t>
+  </si>
+  <si>
+    <t>We divided the remaining sections of the homework and worked on it individually. Later on we collated all our findings in the report.</t>
+  </si>
+  <si>
+    <t>1pm - 6pm</t>
+  </si>
+  <si>
+    <t>Looking for the social context was not difficult as h2 maintains good documentation in their website
+Understood the importance of having proper comments and explanation in the pull requests as it helped in understanding the decisions made by the contributors and the rationale behind each change</t>
+  </si>
+  <si>
+    <t>Happy to complete the homework early</t>
+  </si>
+  <si>
+    <t>9pm - 12am</t>
   </si>
 </sst>
 </file>
@@ -928,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D48" zoomScale="120" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,14 +1756,28 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8"/>
+    <row r="51" spans="1:7" ht="249.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="10">
+        <v>43881</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
@@ -1727,14 +1788,28 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8"/>
+    <row r="53" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A53" s="10">
+        <v>43884</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
@@ -1745,14 +1820,28 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="8"/>
+    <row r="55" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A55" s="10">
+        <v>43885</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>

</xml_diff>

<commit_message>
Checking in diary entry for week 9
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13116804-7342-4717-A6AE-6EA63837BD4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890E29ED-FF62-4746-8AE1-6E0A362D9538}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="158">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -470,6 +470,77 @@
   </si>
   <si>
     <t>9pm - 12am</t>
+  </si>
+  <si>
+    <t>Learn about design patterns</t>
+  </si>
+  <si>
+    <t>Learned 3 more key expert practices and design patterns
+It was really inspiring to hear the experiences of Alberto</t>
+  </si>
+  <si>
+    <t>Understood how we can make use of design patterns to effectively solve a software design problem and how it helps to structure the codebase in a better way which in turn can improve the readbility of the code</t>
+  </si>
+  <si>
+    <t>Wish we could spend more time on design patterns and do some practice on that</t>
+  </si>
+  <si>
+    <t>Discuss this week's homework</t>
+  </si>
+  <si>
+    <t>5pm-7pm</t>
+  </si>
+  <si>
+    <t>Need to find more simpler issues for the  first issue to fix</t>
+  </si>
+  <si>
+    <t>Understood the importance of having proper naming conventions for classes as it helped in narrowing down the design patterns used. For example there was a class names "SessionFactory" which was a clear indicator of the Factory pattern</t>
+  </si>
+  <si>
+    <t>5pm-9pm</t>
+  </si>
+  <si>
+    <t>Identify a simple issue and fix it</t>
+  </si>
+  <si>
+    <t>9pm-12pm</t>
+  </si>
+  <si>
+    <t>Happy to have narrowed down an issue for the first assignment that everyone understood</t>
+  </si>
+  <si>
+    <t>Looked for couple of more simple issues to fix . Found one issue which all of us could understand properly. Started making code changes</t>
+  </si>
+  <si>
+    <t>Submit the pull request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We realized that certain issues that we thought to be easy were actually not that easy to fix due to either lack of proper test cases or complex dependencies in the codebase. </t>
+  </si>
+  <si>
+    <t>The issue was easier to understand because 1)  it was a relatively simple change and had lesser dependencies  2) comments in the pull request were really helpful.</t>
+  </si>
+  <si>
+    <t>Coding the issue was not difficult as we had already discussed the scenarios properly and noted down the various conditions that needs to be covered</t>
+  </si>
+  <si>
+    <t>Hoping that our pull request will get accepted</t>
+  </si>
+  <si>
+    <t>Completed the code changes, tested it and submitted the pull request
+Finished the report</t>
+  </si>
+  <si>
+    <t>Find 5 design patterns in the code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tried to understand various design patterns by going through websites and YouTube videos. Identified 5 design patterns in the codebase and documented the same - Factory, Singleton, Adaptor, Decorator and Command </t>
+  </si>
+  <si>
+    <t>Happy to have identified 5 patterns</t>
+  </si>
+  <si>
+    <t>As Aman and Vaishakhi were not present in the last class, I explained this week's homework. We also discussed couple of possible issues to fix.</t>
   </si>
 </sst>
 </file>
@@ -975,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1852,14 +1923,28 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="8"/>
+    <row r="57" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="10">
+        <v>43888</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
@@ -1870,14 +1955,28 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="8"/>
+    <row r="59" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="10">
+        <v>43890</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
@@ -1888,14 +1987,28 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="8"/>
+    <row r="61" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="10">
+        <v>43891</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
@@ -1906,14 +2019,28 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="8"/>
+    <row r="63" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A63" s="10">
+        <v>43892</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
@@ -1924,14 +2051,28 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="8"/>
+    <row r="65" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A65" s="10">
+        <v>43894</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
@@ -1943,7 +2084,7 @@
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="7"/>
+      <c r="A67" s="10"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>

</xml_diff>